<commit_message>
update prize pool list
</commit_message>
<xml_diff>
--- a/leaderboardpayouts/config/leaderboardpayouts.xlsx
+++ b/leaderboardpayouts/config/leaderboardpayouts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="20% paid" sheetId="1" state="visible" r:id="rId2"/>
@@ -263,7 +263,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -285,34 +285,34 @@
       <sz val="8"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FFAF192D"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Cambria"/>
-      <family val="0"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
-      <family val="0"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -500,26 +500,26 @@
   </sheetPr>
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H5" activeCellId="0" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="AC2" activeCellId="0" sqref="AC2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="3" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="12" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="6.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="23" style="0" width="5.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="4.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="3.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="30" style="0" width="14.43"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="10" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="21" min="12" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="27" min="23" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="14.1734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -609,752 +609,752 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>15.5</v>
+        <v>1550</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>16</v>
+        <v>1600</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>16.5</v>
+        <v>1650</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>17</v>
+        <v>1700</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>17.5</v>
+        <v>1750</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>18</v>
+        <v>1800</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>18.5</v>
+        <v>1850</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>19</v>
+        <v>1900</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>19.5</v>
+        <v>1950</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>20</v>
+        <v>2000</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>20.5</v>
+        <v>2050</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>21</v>
+        <v>2100</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>21.5</v>
+        <v>2150</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>22</v>
+        <v>2200</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>22.5</v>
+        <v>2250</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>23</v>
+        <v>2300</v>
       </c>
       <c r="R2" s="2" t="n">
-        <v>24</v>
+        <v>2400</v>
       </c>
       <c r="S2" s="2" t="n">
-        <v>25</v>
+        <v>2400</v>
       </c>
       <c r="T2" s="2" t="n">
-        <v>26</v>
+        <v>2600</v>
       </c>
       <c r="U2" s="2" t="n">
-        <v>27</v>
+        <v>2700</v>
       </c>
       <c r="V2" s="2" t="n">
-        <v>28</v>
+        <v>2800</v>
       </c>
       <c r="W2" s="2" t="n">
-        <v>29</v>
+        <v>2900</v>
       </c>
       <c r="X2" s="2" t="n">
-        <v>31</v>
+        <v>3100</v>
       </c>
       <c r="Y2" s="2" t="n">
-        <v>33</v>
+        <v>3300</v>
       </c>
       <c r="Z2" s="2" t="n">
-        <v>35</v>
+        <v>3500</v>
       </c>
       <c r="AA2" s="2" t="n">
-        <v>40</v>
+        <v>4000</v>
       </c>
       <c r="AB2" s="2" t="n">
-        <v>70</v>
+        <v>7000</v>
       </c>
       <c r="AC2" s="2" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>10.75</v>
+        <v>1075</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>11</v>
+        <v>1100</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>11.25</v>
+        <v>1125</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>11.5</v>
+        <v>1150</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>11.75</v>
+        <v>1175</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>12</v>
+        <v>1200</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>12.25</v>
+        <v>1225</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>12.5</v>
+        <v>1250</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>12.75</v>
+        <v>1275</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>13</v>
+        <v>1300</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>13.25</v>
+        <v>1325</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>13.5</v>
+        <v>1350</v>
       </c>
       <c r="N3" s="2" t="n">
-        <v>13.75</v>
+        <v>1375</v>
       </c>
       <c r="O3" s="2" t="n">
-        <v>14</v>
+        <v>1400</v>
       </c>
       <c r="P3" s="2" t="n">
-        <v>14.25</v>
+        <v>1425</v>
       </c>
       <c r="Q3" s="2" t="n">
-        <v>14.5</v>
+        <v>1450</v>
       </c>
       <c r="R3" s="2" t="n">
-        <v>15</v>
+        <v>1500</v>
       </c>
       <c r="S3" s="2" t="n">
-        <v>15.5</v>
+        <v>1550</v>
       </c>
       <c r="T3" s="2" t="n">
-        <v>16</v>
+        <v>1600</v>
       </c>
       <c r="U3" s="2" t="n">
-        <v>16.5</v>
+        <v>1650</v>
       </c>
       <c r="V3" s="2" t="n">
-        <v>17</v>
+        <v>1700</v>
       </c>
       <c r="W3" s="2" t="n">
-        <v>17.5</v>
+        <v>1750</v>
       </c>
       <c r="X3" s="2" t="n">
-        <v>19</v>
+        <v>1900</v>
       </c>
       <c r="Y3" s="2" t="n">
-        <v>20</v>
+        <v>2000</v>
       </c>
       <c r="Z3" s="2" t="n">
-        <v>22</v>
+        <v>2200</v>
       </c>
       <c r="AA3" s="2" t="n">
-        <v>25</v>
+        <v>2500</v>
       </c>
       <c r="AB3" s="2" t="n">
-        <v>30</v>
+        <v>3000</v>
       </c>
       <c r="AC3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>6.4</v>
+        <v>640</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>6.4</v>
+        <v>640</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>6.6</v>
+        <v>660</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>6.6</v>
+        <v>660</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>6.7</v>
+        <v>670</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>6.8</v>
+        <v>680</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>6.9</v>
+        <v>690</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>6.9</v>
+        <v>690</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>7</v>
+        <v>700</v>
       </c>
       <c r="K4" s="2" t="n">
-        <v>7.2</v>
+        <v>720</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>7.2</v>
+        <v>720</v>
       </c>
       <c r="M4" s="2" t="n">
-        <v>7.4</v>
+        <v>740</v>
       </c>
       <c r="N4" s="2" t="n">
-        <v>7.4</v>
+        <v>740</v>
       </c>
       <c r="O4" s="2" t="n">
-        <v>7.5</v>
+        <v>750</v>
       </c>
       <c r="P4" s="2" t="n">
-        <v>7.6</v>
+        <v>760</v>
       </c>
       <c r="Q4" s="2" t="n">
-        <v>7.7</v>
+        <v>770</v>
       </c>
       <c r="R4" s="2" t="n">
-        <v>7.8</v>
+        <v>780</v>
       </c>
       <c r="S4" s="2" t="n">
-        <v>7.9</v>
+        <v>790</v>
       </c>
       <c r="T4" s="2" t="n">
-        <v>8.1</v>
+        <v>810</v>
       </c>
       <c r="U4" s="2" t="n">
-        <v>8.2</v>
+        <v>820</v>
       </c>
       <c r="V4" s="2" t="n">
-        <v>8.4</v>
+        <v>840</v>
       </c>
       <c r="W4" s="2" t="n">
-        <v>8.9</v>
+        <v>890</v>
       </c>
       <c r="X4" s="2" t="n">
-        <v>9.8</v>
+        <v>980</v>
       </c>
       <c r="Y4" s="2" t="n">
-        <v>12</v>
+        <v>1200</v>
       </c>
       <c r="Z4" s="2" t="n">
-        <v>15</v>
+        <v>1500</v>
       </c>
       <c r="AA4" s="2" t="n">
-        <v>20</v>
+        <v>2000</v>
       </c>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>5.4</v>
+        <v>540</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>5.4</v>
+        <v>540</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>5.6</v>
+        <v>560</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>5.6</v>
+        <v>560</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>5.7</v>
+        <v>570</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>5.8</v>
+        <v>580</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>5.9</v>
+        <v>590</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>5.9</v>
+        <v>590</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>6</v>
+        <v>600</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>6.2</v>
+        <v>620</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>6.2</v>
+        <v>620</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>6.4</v>
+        <v>640</v>
       </c>
       <c r="N5" s="2" t="n">
-        <v>6.4</v>
+        <v>640</v>
       </c>
       <c r="O5" s="2" t="n">
-        <v>6.5</v>
+        <v>650</v>
       </c>
       <c r="P5" s="2" t="n">
-        <v>6.6</v>
+        <v>660</v>
       </c>
       <c r="Q5" s="2" t="n">
-        <v>6.7</v>
+        <v>670</v>
       </c>
       <c r="R5" s="2" t="n">
-        <v>6.8</v>
+        <v>680</v>
       </c>
       <c r="S5" s="2" t="n">
-        <v>6.9</v>
+        <v>690</v>
       </c>
       <c r="T5" s="2" t="n">
-        <v>7.1</v>
+        <v>710</v>
       </c>
       <c r="U5" s="2" t="n">
-        <v>7.2</v>
+        <v>720</v>
       </c>
       <c r="V5" s="2" t="n">
-        <v>7.5</v>
+        <v>750</v>
       </c>
       <c r="W5" s="2" t="n">
-        <v>7.9</v>
+        <v>790</v>
       </c>
       <c r="X5" s="2" t="n">
-        <v>8.8</v>
+        <v>880</v>
       </c>
       <c r="Y5" s="2" t="n">
-        <v>9</v>
+        <v>900</v>
       </c>
       <c r="Z5" s="2" t="n">
-        <v>11</v>
+        <v>1100</v>
       </c>
       <c r="AA5" s="2" t="n">
-        <v>15</v>
+        <v>1500</v>
       </c>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>4.4</v>
+        <v>440</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>4.4</v>
+        <v>440</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>4.6</v>
+        <v>460</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>4.6</v>
+        <v>460</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>4.7</v>
+        <v>470</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>4.8</v>
+        <v>480</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>4.9</v>
+        <v>490</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>4.9</v>
+        <v>490</v>
       </c>
       <c r="J6" s="2" t="n">
-        <v>5</v>
+        <v>500</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>5.2</v>
+        <v>520</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>5.2</v>
+        <v>520</v>
       </c>
       <c r="M6" s="2" t="n">
-        <v>5.4</v>
+        <v>540</v>
       </c>
       <c r="N6" s="2" t="n">
-        <v>5.4</v>
+        <v>540</v>
       </c>
       <c r="O6" s="2" t="n">
-        <v>5.5</v>
+        <v>550</v>
       </c>
       <c r="P6" s="2" t="n">
-        <v>5.6</v>
+        <v>560</v>
       </c>
       <c r="Q6" s="2" t="n">
-        <v>5.7</v>
+        <v>570</v>
       </c>
       <c r="R6" s="2" t="n">
-        <v>5.8</v>
+        <v>580</v>
       </c>
       <c r="S6" s="2" t="n">
-        <v>5.9</v>
+        <v>590</v>
       </c>
       <c r="T6" s="2" t="n">
-        <v>6.1</v>
+        <v>610</v>
       </c>
       <c r="U6" s="2" t="n">
-        <v>6.2</v>
+        <v>620</v>
       </c>
       <c r="V6" s="2" t="n">
-        <v>6.5</v>
+        <v>650</v>
       </c>
       <c r="W6" s="2" t="n">
-        <v>6.9</v>
+        <v>690</v>
       </c>
       <c r="X6" s="2" t="n">
-        <v>7.8</v>
+        <v>780</v>
       </c>
       <c r="Y6" s="2" t="n">
-        <v>8</v>
+        <v>800</v>
       </c>
       <c r="Z6" s="2" t="n">
-        <v>9</v>
+        <v>900</v>
       </c>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>3.4</v>
+        <v>340</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>3.4</v>
+        <v>340</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>3.5</v>
+        <v>350</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>3.5</v>
+        <v>350</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>3.6</v>
+        <v>360</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>3.7</v>
+        <v>370</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>3.8</v>
+        <v>380</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>3.8</v>
+        <v>380</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>4</v>
+        <v>400</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>4.2</v>
+        <v>420</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>4.2</v>
+        <v>420</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>4.4</v>
+        <v>440</v>
       </c>
       <c r="N7" s="2" t="n">
-        <v>4.4</v>
+        <v>440</v>
       </c>
       <c r="O7" s="2" t="n">
-        <v>4.5</v>
+        <v>450</v>
       </c>
       <c r="P7" s="2" t="n">
-        <v>4.6</v>
+        <v>460</v>
       </c>
       <c r="Q7" s="2" t="n">
-        <v>4.7</v>
+        <v>470</v>
       </c>
       <c r="R7" s="2" t="n">
-        <v>4.8</v>
+        <v>480</v>
       </c>
       <c r="S7" s="2" t="n">
-        <v>4.9</v>
+        <v>490</v>
       </c>
       <c r="T7" s="2" t="n">
-        <v>5.1</v>
+        <v>510</v>
       </c>
       <c r="U7" s="2" t="n">
-        <v>5.2</v>
+        <v>520</v>
       </c>
       <c r="V7" s="2" t="n">
-        <v>5.5</v>
+        <v>550</v>
       </c>
       <c r="W7" s="2" t="n">
-        <v>5.9</v>
+        <v>590</v>
       </c>
       <c r="X7" s="2" t="n">
-        <v>6.8</v>
+        <v>680</v>
       </c>
       <c r="Y7" s="2" t="n">
-        <v>7</v>
+        <v>700</v>
       </c>
       <c r="Z7" s="2" t="n">
-        <v>8</v>
+        <v>800</v>
       </c>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>2.3</v>
+        <v>230</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>2.3</v>
+        <v>230</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>2.4</v>
+        <v>240</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>2.4</v>
+        <v>240</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>2.5</v>
+        <v>250</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>2.6</v>
+        <v>260</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>2.7</v>
+        <v>270</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>2.7</v>
+        <v>270</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>2.8</v>
+        <v>280</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>3.2</v>
+        <v>320</v>
       </c>
       <c r="N8" s="2" t="n">
-        <v>3.2</v>
+        <v>320</v>
       </c>
       <c r="O8" s="2" t="n">
-        <v>3.3</v>
+        <v>330</v>
       </c>
       <c r="P8" s="2" t="n">
-        <v>3.4</v>
+        <v>340</v>
       </c>
       <c r="Q8" s="2" t="n">
-        <v>3.5</v>
+        <v>350</v>
       </c>
       <c r="R8" s="2" t="n">
-        <v>3.6</v>
+        <v>360</v>
       </c>
       <c r="S8" s="2" t="n">
-        <v>3.7</v>
+        <v>370</v>
       </c>
       <c r="T8" s="2" t="n">
-        <v>3.9</v>
+        <v>390</v>
       </c>
       <c r="U8" s="2" t="n">
-        <v>4</v>
+        <v>400</v>
       </c>
       <c r="V8" s="2" t="n">
-        <v>4.3</v>
+        <v>430</v>
       </c>
       <c r="W8" s="2" t="n">
-        <v>4.7</v>
+        <v>470</v>
       </c>
       <c r="X8" s="2" t="n">
-        <v>5.5</v>
+        <v>550</v>
       </c>
       <c r="Y8" s="2" t="n">
-        <v>6</v>
+        <v>600</v>
       </c>
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>1.3</v>
+        <v>130</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>1.3</v>
+        <v>130</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>1.4</v>
+        <v>140</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>1.4</v>
+        <v>140</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>1.4</v>
+        <v>140</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>1.5</v>
+        <v>150</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>1.6</v>
+        <v>160</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>1.6</v>
+        <v>160</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>1.7</v>
+        <v>170</v>
       </c>
       <c r="K9" s="2" t="n">
-        <v>1.8</v>
+        <v>180</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>1.8</v>
+        <v>180</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>1.9</v>
+        <v>190</v>
       </c>
       <c r="N9" s="2" t="n">
-        <v>1.9</v>
+        <v>190</v>
       </c>
       <c r="O9" s="2" t="n">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="P9" s="2" t="n">
-        <v>2.1</v>
+        <v>210</v>
       </c>
       <c r="Q9" s="2" t="n">
-        <v>2.2</v>
+        <v>220</v>
       </c>
       <c r="R9" s="2" t="n">
-        <v>2.3</v>
+        <v>230</v>
       </c>
       <c r="S9" s="2" t="n">
-        <v>2.4</v>
+        <v>240</v>
       </c>
       <c r="T9" s="2" t="n">
-        <v>2.6</v>
+        <v>260</v>
       </c>
       <c r="U9" s="2" t="n">
-        <v>2.7</v>
+        <v>270</v>
       </c>
       <c r="V9" s="2" t="n">
-        <v>2.9</v>
+        <v>290</v>
       </c>
       <c r="W9" s="2" t="n">
-        <v>3.5</v>
+        <v>350</v>
       </c>
       <c r="X9" s="2" t="n">
-        <v>4.4</v>
+        <v>440</v>
       </c>
       <c r="Y9" s="2" t="n">
-        <v>5</v>
+        <v>500</v>
       </c>
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.95</v>
+        <v>95</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0.95</v>
+        <v>95</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>1.1</v>
+        <v>110</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>1.2</v>
+        <v>120</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>1.2</v>
+        <v>120</v>
       </c>
       <c r="J10" s="2" t="n">
-        <v>1.3</v>
+        <v>130</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>1.5</v>
+        <v>150</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>1.5</v>
+        <v>150</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>1.6</v>
+        <v>160</v>
       </c>
       <c r="N10" s="2" t="n">
-        <v>1.6</v>
+        <v>160</v>
       </c>
       <c r="O10" s="2" t="n">
-        <v>1.7</v>
+        <v>170</v>
       </c>
       <c r="P10" s="2" t="n">
-        <v>1.8</v>
+        <v>180</v>
       </c>
       <c r="Q10" s="2" t="n">
-        <v>1.9</v>
+        <v>190</v>
       </c>
       <c r="R10" s="2" t="n">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="S10" s="2" t="n">
-        <v>2.1</v>
+        <v>210</v>
       </c>
       <c r="T10" s="2" t="n">
-        <v>2.3</v>
+        <v>230</v>
       </c>
       <c r="U10" s="2" t="n">
-        <v>2.4</v>
+        <v>240</v>
       </c>
       <c r="V10" s="2" t="n">
-        <v>2.6</v>
+        <v>260</v>
       </c>
       <c r="W10" s="2" t="n">
-        <v>2.9</v>
+        <v>290</v>
       </c>
       <c r="X10" s="2" t="n">
-        <v>3.7</v>
+        <v>370</v>
       </c>
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
@@ -1362,78 +1362,78 @@
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.75</v>
+        <v>75</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0.75</v>
+        <v>75</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>0.95</v>
+        <v>95</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>0.95</v>
+        <v>95</v>
       </c>
       <c r="J11" s="2" t="n">
-        <v>1.05</v>
+        <v>105</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>1.1</v>
+        <v>110</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>1.1</v>
+        <v>110</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>1.15</v>
+        <v>115</v>
       </c>
       <c r="N11" s="2" t="n">
-        <v>1.15</v>
+        <v>115</v>
       </c>
       <c r="O11" s="2" t="n">
-        <v>1.2</v>
+        <v>120</v>
       </c>
       <c r="P11" s="2" t="n">
-        <v>1.25</v>
+        <v>125</v>
       </c>
       <c r="Q11" s="2" t="n">
-        <v>1.3</v>
+        <v>130</v>
       </c>
       <c r="R11" s="2" t="n">
-        <v>1.4</v>
+        <v>140</v>
       </c>
       <c r="S11" s="2" t="n">
-        <v>1.45</v>
+        <v>145</v>
       </c>
       <c r="T11" s="2" t="n">
-        <v>1.55</v>
+        <v>150</v>
       </c>
       <c r="U11" s="2" t="n">
-        <v>1.6</v>
+        <v>160</v>
       </c>
       <c r="V11" s="2" t="n">
-        <v>1.8</v>
+        <v>180</v>
       </c>
       <c r="W11" s="2" t="n">
-        <v>2.3</v>
+        <v>230</v>
       </c>
       <c r="X11" s="2" t="n">
-        <v>3.2</v>
+        <v>320</v>
       </c>
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
@@ -1441,75 +1441,75 @@
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
         <v>15</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.75</v>
+        <v>75</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0.75</v>
+        <v>75</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>0.95</v>
+        <v>95</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>0.95</v>
+        <v>95</v>
       </c>
       <c r="J12" s="2" t="n">
-        <v>1.05</v>
+        <v>105</v>
       </c>
       <c r="K12" s="2" t="n">
-        <v>1.1</v>
+        <v>110</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>1.1</v>
+        <v>110</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>1.15</v>
+        <v>115</v>
       </c>
       <c r="N12" s="2" t="n">
-        <v>1.15</v>
+        <v>115</v>
       </c>
       <c r="O12" s="2" t="n">
-        <v>1.2</v>
+        <v>120</v>
       </c>
       <c r="P12" s="2" t="n">
-        <v>1.25</v>
+        <v>125</v>
       </c>
       <c r="Q12" s="2" t="n">
-        <v>1.3</v>
+        <v>130</v>
       </c>
       <c r="R12" s="2" t="n">
-        <v>1.4</v>
+        <v>140</v>
       </c>
       <c r="S12" s="2" t="n">
-        <v>1.45</v>
+        <v>145</v>
       </c>
       <c r="T12" s="2" t="n">
-        <v>1.55</v>
+        <v>155</v>
       </c>
       <c r="U12" s="2" t="n">
-        <v>1.6</v>
+        <v>160</v>
       </c>
       <c r="V12" s="2" t="n">
-        <v>1.8</v>
+        <v>180</v>
       </c>
       <c r="W12" s="2" t="n">
-        <v>2.1</v>
+        <v>210</v>
       </c>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
@@ -1518,72 +1518,72 @@
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
         <v>20</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>0.35</v>
+        <v>35</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>0.35</v>
+        <v>35</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>0.35</v>
+        <v>35</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>0.45</v>
+        <v>45</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>0.45</v>
+        <v>45</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>0.55</v>
+        <v>55</v>
       </c>
       <c r="J13" s="2" t="n">
-        <v>0.6</v>
+        <v>60</v>
       </c>
       <c r="K13" s="2" t="n">
-        <v>0.6</v>
+        <v>60</v>
       </c>
       <c r="L13" s="2" t="n">
-        <v>0.6</v>
+        <v>60</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>0.65</v>
+        <v>65</v>
       </c>
       <c r="N13" s="2" t="n">
-        <v>0.7</v>
+        <v>70</v>
       </c>
       <c r="O13" s="2" t="n">
-        <v>0.75</v>
+        <v>75</v>
       </c>
       <c r="P13" s="2" t="n">
-        <v>0.75</v>
+        <v>75</v>
       </c>
       <c r="Q13" s="2" t="n">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="R13" s="2" t="n">
-        <v>0.8</v>
+        <v>80</v>
       </c>
       <c r="S13" s="2" t="n">
-        <v>0.95</v>
+        <v>95</v>
       </c>
       <c r="T13" s="2" t="n">
-        <v>1.05</v>
+        <v>105</v>
       </c>
       <c r="U13" s="2" t="n">
-        <v>1.15</v>
+        <v>115</v>
       </c>
       <c r="V13" s="2" t="n">
-        <v>1.3</v>
+        <v>130</v>
       </c>
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
@@ -1593,69 +1593,69 @@
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>25</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>0.3</v>
+        <v>30</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>0.3</v>
+        <v>30</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>0.3</v>
+        <v>30</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>0.35</v>
+        <v>35</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>0.35</v>
+        <v>35</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>0.4</v>
+        <v>40</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>0.4</v>
+        <v>40</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>0.45</v>
+        <v>45</v>
       </c>
       <c r="J14" s="2" t="n">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="K14" s="2" t="n">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="L14" s="2" t="n">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="M14" s="2" t="n">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="N14" s="2" t="n">
-        <v>0.55</v>
+        <v>55</v>
       </c>
       <c r="O14" s="2" t="n">
-        <v>0.6</v>
+        <v>60</v>
       </c>
       <c r="P14" s="2" t="n">
-        <v>0.65</v>
+        <v>65</v>
       </c>
       <c r="Q14" s="2" t="n">
-        <v>0.7</v>
+        <v>70</v>
       </c>
       <c r="R14" s="2" t="n">
-        <v>0.7</v>
+        <v>70</v>
       </c>
       <c r="S14" s="2" t="n">
-        <v>0.75</v>
+        <v>75</v>
       </c>
       <c r="T14" s="2" t="n">
-        <v>0.9</v>
+        <v>90</v>
       </c>
       <c r="U14" s="2" t="n">
-        <v>1.05</v>
+        <v>105</v>
       </c>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -1666,66 +1666,66 @@
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <v>30</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>0.2</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>0.2</v>
+        <v>20</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>0.2</v>
+        <v>20</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>0.25</v>
+        <v>25</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>0.25</v>
+        <v>25</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>0.3</v>
+        <v>30</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>0.3</v>
+        <v>30</v>
       </c>
       <c r="I15" s="2" t="n">
-        <v>0.35</v>
+        <v>35</v>
       </c>
       <c r="J15" s="2" t="n">
-        <v>0.4</v>
+        <v>40</v>
       </c>
       <c r="K15" s="2" t="n">
-        <v>0.4</v>
+        <v>40</v>
       </c>
       <c r="L15" s="2" t="n">
-        <v>0.4</v>
+        <v>40</v>
       </c>
       <c r="M15" s="2" t="n">
-        <v>0.4</v>
+        <v>40</v>
       </c>
       <c r="N15" s="2" t="n">
-        <v>0.45</v>
+        <v>45</v>
       </c>
       <c r="O15" s="2" t="n">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="P15" s="2" t="n">
-        <v>0.55</v>
+        <v>55</v>
       </c>
       <c r="Q15" s="2" t="n">
-        <v>0.55</v>
+        <v>55</v>
       </c>
       <c r="R15" s="2" t="n">
-        <v>0.55</v>
+        <v>55</v>
       </c>
       <c r="S15" s="2" t="n">
-        <v>0.6</v>
+        <v>60</v>
       </c>
       <c r="T15" s="2" t="n">
-        <v>0.75</v>
+        <v>75</v>
       </c>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
@@ -1737,63 +1737,63 @@
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <v>35</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>0.19</v>
+        <v>19</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>0.19</v>
+        <v>19</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>0.19</v>
+        <v>19</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>0.2</v>
+        <v>20</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>0.2</v>
+        <v>20</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>0.2</v>
+        <v>20</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>0.2</v>
+        <v>20</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>0.25</v>
+        <v>25</v>
       </c>
       <c r="J16" s="2" t="n">
-        <v>0.3</v>
+        <v>30</v>
       </c>
       <c r="K16" s="2" t="n">
-        <v>0.3</v>
+        <v>30</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>0.3</v>
+        <v>30</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>0.3</v>
+        <v>30</v>
       </c>
       <c r="N16" s="2" t="n">
-        <v>0.35</v>
+        <v>35</v>
       </c>
       <c r="O16" s="2" t="n">
-        <v>0.4</v>
+        <v>40</v>
       </c>
       <c r="P16" s="2" t="n">
-        <v>0.45</v>
+        <v>45</v>
       </c>
       <c r="Q16" s="2" t="n">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="R16" s="2" t="n">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="S16" s="2" t="n">
-        <v>0.55</v>
+        <v>55</v>
       </c>
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
@@ -1806,63 +1806,63 @@
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
         <v>40</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>0.16</v>
+        <v>16</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>0.16</v>
+        <v>16</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0.16</v>
+        <v>16</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>0.18</v>
+        <v>18</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>0.18</v>
+        <v>18</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>0.18</v>
+        <v>18</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>0.18</v>
+        <v>18</v>
       </c>
       <c r="I17" s="2" t="n">
-        <v>0.21</v>
+        <v>21</v>
       </c>
       <c r="J17" s="2" t="n">
-        <v>0.25</v>
+        <v>25</v>
       </c>
       <c r="K17" s="2" t="n">
-        <v>0.25</v>
+        <v>25</v>
       </c>
       <c r="L17" s="2" t="n">
-        <v>0.25</v>
+        <v>25</v>
       </c>
       <c r="M17" s="2" t="n">
-        <v>0.25</v>
+        <v>25</v>
       </c>
       <c r="N17" s="2" t="n">
-        <v>0.3</v>
+        <v>30</v>
       </c>
       <c r="O17" s="2" t="n">
-        <v>0.35</v>
+        <v>35</v>
       </c>
       <c r="P17" s="2" t="n">
-        <v>0.4</v>
+        <v>40</v>
       </c>
       <c r="Q17" s="2" t="n">
-        <v>0.45</v>
+        <v>45</v>
       </c>
       <c r="R17" s="2" t="n">
-        <v>0.45</v>
+        <v>45</v>
       </c>
       <c r="S17" s="2" t="n">
-        <v>0.55</v>
+        <v>55</v>
       </c>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
@@ -1875,60 +1875,60 @@
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
         <v>50</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>0.15</v>
+        <v>15</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>0.15</v>
+        <v>15</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>0.15</v>
+        <v>15</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>0.16</v>
+        <v>16</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>0.16</v>
+        <v>16</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>0.17</v>
+        <v>17</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>0.17</v>
+        <v>17</v>
       </c>
       <c r="I18" s="2" t="n">
-        <v>0.18</v>
+        <v>18</v>
       </c>
       <c r="J18" s="2" t="n">
-        <v>0.21</v>
+        <v>21</v>
       </c>
       <c r="K18" s="2" t="n">
-        <v>0.21</v>
+        <v>21</v>
       </c>
       <c r="L18" s="2" t="n">
-        <v>0.21</v>
+        <v>21</v>
       </c>
       <c r="M18" s="2" t="n">
-        <v>0.21</v>
+        <v>21</v>
       </c>
       <c r="N18" s="2" t="n">
-        <v>0.25</v>
+        <v>25</v>
       </c>
       <c r="O18" s="2" t="n">
-        <v>0.31</v>
+        <v>31</v>
       </c>
       <c r="P18" s="2" t="n">
-        <v>0.35</v>
+        <v>35</v>
       </c>
       <c r="Q18" s="2" t="n">
-        <v>0.4</v>
+        <v>40</v>
       </c>
       <c r="R18" s="2" t="n">
-        <v>0.45</v>
+        <v>45</v>
       </c>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
@@ -1942,57 +1942,57 @@
       <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
         <v>60</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>0.14</v>
+        <v>14</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>0.14</v>
+        <v>14</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>0.14</v>
+        <v>14</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>0.14</v>
+        <v>14</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>0.14</v>
+        <v>14</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>0.15</v>
+        <v>15</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>0.15</v>
+        <v>15</v>
       </c>
       <c r="I19" s="2" t="n">
-        <v>0.17</v>
+        <v>17</v>
       </c>
       <c r="J19" s="2" t="n">
-        <v>0.18</v>
+        <v>18</v>
       </c>
       <c r="K19" s="2" t="n">
-        <v>0.18</v>
+        <v>18</v>
       </c>
       <c r="L19" s="2" t="n">
-        <v>0.19</v>
+        <v>19</v>
       </c>
       <c r="M19" s="2" t="n">
-        <v>0.19</v>
+        <v>19</v>
       </c>
       <c r="N19" s="2" t="n">
-        <v>0.22</v>
+        <v>22</v>
       </c>
       <c r="O19" s="2" t="n">
-        <v>0.26</v>
+        <v>26</v>
       </c>
       <c r="P19" s="2" t="n">
-        <v>0.31</v>
+        <v>31</v>
       </c>
       <c r="Q19" s="2" t="n">
-        <v>0.33</v>
+        <v>33</v>
       </c>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
@@ -2007,54 +2007,54 @@
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
         <v>75</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>0.13</v>
+        <v>13</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>0.13</v>
+        <v>13</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>0.13</v>
+        <v>13</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>0.13</v>
+        <v>13</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>0.13</v>
+        <v>13</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>0.13</v>
+        <v>13</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>0.13</v>
+        <v>13</v>
       </c>
       <c r="I20" s="2" t="n">
-        <v>0.15</v>
+        <v>15</v>
       </c>
       <c r="J20" s="2" t="n">
-        <v>0.15</v>
+        <v>15</v>
       </c>
       <c r="K20" s="2" t="n">
-        <v>0.16</v>
+        <v>16</v>
       </c>
       <c r="L20" s="2" t="n">
-        <v>0.17</v>
+        <v>17</v>
       </c>
       <c r="M20" s="2" t="n">
-        <v>0.17</v>
+        <v>17</v>
       </c>
       <c r="N20" s="2" t="n">
-        <v>0.19</v>
+        <v>19</v>
       </c>
       <c r="O20" s="2" t="n">
-        <v>0.19</v>
+        <v>19</v>
       </c>
       <c r="P20" s="3" t="n">
-        <v>0.23</v>
+        <v>23</v>
       </c>
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
@@ -2062,251 +2062,251 @@
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
         <v>100</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>0.12</v>
+        <v>12</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>0.12</v>
+        <v>12</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>0.12</v>
+        <v>12</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>0.12</v>
+        <v>12</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>0.12</v>
+        <v>12</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>0.12</v>
+        <v>12</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>0.12</v>
+        <v>12</v>
       </c>
       <c r="I21" s="2" t="n">
-        <v>0.12</v>
+        <v>12</v>
       </c>
       <c r="J21" s="2" t="n">
-        <v>0.12</v>
+        <v>12</v>
       </c>
       <c r="K21" s="2" t="n">
-        <v>0.13</v>
+        <v>13</v>
       </c>
       <c r="L21" s="2" t="n">
-        <v>0.15</v>
+        <v>15</v>
       </c>
       <c r="M21" s="2" t="n">
-        <v>0.16</v>
+        <v>16</v>
       </c>
       <c r="N21" s="2" t="n">
-        <v>0.17</v>
+        <v>17</v>
       </c>
       <c r="O21" s="2" t="n">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
         <v>125</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="I22" s="2" t="n">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="J22" s="2" t="n">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="K22" s="2" t="n">
-        <v>0.12</v>
+        <v>12</v>
       </c>
       <c r="L22" s="2" t="n">
-        <v>0.14</v>
+        <v>14</v>
       </c>
       <c r="M22" s="2" t="n">
-        <v>0.15</v>
+        <v>15</v>
       </c>
       <c r="N22" s="2" t="n">
-        <v>0.16</v>
+        <v>16</v>
       </c>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
         <v>150</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>0.1</v>
+        <v>11</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="I23" s="2" t="n">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="J23" s="2" t="n">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.12</v>
+        <v>12</v>
       </c>
       <c r="L23" s="2" t="n">
-        <v>0.13</v>
+        <v>13</v>
       </c>
       <c r="M23" s="2" t="n">
-        <v>0.14</v>
+        <v>14</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
         <v>175</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="I24" s="2" t="n">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="J24" s="2" t="n">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="K24" s="2" t="n">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="L24" s="2" t="n">
-        <v>0.13</v>
+        <v>13</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
         <v>200</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="I25" s="2" t="n">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="J25" s="2" t="n">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="K25" s="2" t="n">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
         <v>225</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>0.07</v>
+        <v>7</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>0.07</v>
+        <v>7</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>0.07</v>
+        <v>7</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>0.07</v>
+        <v>7</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>0.07</v>
+        <v>7</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>0.07</v>
+        <v>7</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="I26" s="2" t="n">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="J26" s="2" t="n">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
@@ -2314,36 +2314,36 @@
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
         <v>250</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>0.07</v>
+        <v>7</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>0.07</v>
+        <v>7</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>0.07</v>
+        <v>7</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>0.07</v>
+        <v>7</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>0.07</v>
+        <v>7</v>
       </c>
       <c r="H27" s="2" t="n">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="I27" s="2" t="n">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="J27" s="2" t="n">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
@@ -2351,33 +2351,33 @@
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
         <v>275</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>0.07</v>
+        <v>7</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>0.07</v>
+        <v>7</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>0.07</v>
+        <v>7</v>
       </c>
       <c r="I28" s="2" t="n">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
@@ -2386,33 +2386,33 @@
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
         <v>300</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="H29" s="2" t="n">
-        <v>0.07</v>
+        <v>7</v>
       </c>
       <c r="I29" s="2" t="n">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
@@ -2421,30 +2421,30 @@
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
         <v>350</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>0.07</v>
+        <v>7</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -2454,27 +2454,27 @@
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
         <v>400</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -2485,24 +2485,24 @@
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
         <v>450</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>0.04</v>
+        <v>5</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -2514,21 +2514,21 @@
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
         <v>500</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>0.04</v>
+        <v>5</v>
       </c>
       <c r="C33" s="2" t="n">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -2541,18 +2541,18 @@
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
         <v>550</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>0.04</v>
+        <v>5</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -2566,15 +2566,15 @@
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
         <v>600</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>0.04</v>
+        <v>5</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -2589,12 +2589,12 @@
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
         <v>650</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>0.03</v>
+        <v>5</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -2610,12 +2610,12 @@
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
         <v>700</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>0.03</v>
+        <v>5</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -2634,7 +2634,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2649,7 +2649,7 @@
   </sheetPr>
   <dimension ref="A1:AF34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -2657,18 +2657,18 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="3" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="12" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="6.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="25" style="0" width="5.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="4.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="3.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="33" style="0" width="14.43"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="10" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="23" min="12" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="30" min="25" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="4.45408163265306"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="33" style="0" width="14.1734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4794,7 +4794,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4809,7 +4809,7 @@
   </sheetPr>
   <dimension ref="A1:AF34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -4817,18 +4817,18 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="16" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="6.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="26" style="0" width="5.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="4.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="3.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="33" style="0" width="14.43"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="14" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="24" min="16" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="30" min="26" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="4.45408163265306"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="33" style="0" width="14.1734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6944,7 +6944,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6959,13 +6959,13 @@
   </sheetPr>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.43"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.1734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7262,7 +7262,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -7277,13 +7277,13 @@
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.43"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.1734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7409,7 +7409,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -7424,13 +7424,13 @@
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.43"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.1734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7565,7 +7565,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>